<commit_message>
New Transitions and rules
</commit_message>
<xml_diff>
--- a/Transitions.xlsx
+++ b/Transitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soporte\Documents\Proyectos\8vo\TC3002B_Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4533B5B5-29A5-4C00-91E9-9DA293AA0E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{688AA7AA-BD07-4535-B148-A30C1E8D5F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B158C7EA-0D1B-4D7A-B6B3-93370AB3C5AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8BAEB8F-46F8-4565-B617-1B74684AEC82}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -65,10 +65,10 @@
     <t>equal_op</t>
   </si>
   <si>
+    <t>inc_kwd</t>
+  </si>
+  <si>
     <t>dec_kwd</t>
-  </si>
-  <si>
-    <t>inc_kwd</t>
   </si>
   <si>
     <t>if_kwd</t>
@@ -3340,11 +3340,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02EC81D-CB53-4E9B-ABBA-208CCDE8BC9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315E925E-B9AB-406F-BA8F-B3AA1E890C41}">
   <dimension ref="A1:CI152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>